<commit_message>
docs: add timeline image in docs
</commit_message>
<xml_diff>
--- a/docs/boards/sprint_1.xlsx
+++ b/docs/boards/sprint_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEF192A-F11C-487C-831E-A74A28A94A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157483D5-30E6-4E2C-AEB6-A528539EB311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,6 +506,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -532,9 +535,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2793,7 +2793,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>HOURS: 0.30s</a:t>
+            <a:t>HOURS: 0.30</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400" u="none">
             <a:solidFill>
@@ -4878,8 +4878,8 @@
   </sheetPr>
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B9" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4996,50 +4996,50 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="43"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="37"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="38"/>
       <c r="H9" s="9"/>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="44"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="38"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="39"/>
       <c r="H10" s="7"/>
       <c r="J10" s="6"/>
-      <c r="M10" s="46"/>
+      <c r="M10" s="37"/>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="45"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="39"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="40"/>
       <c r="H11" s="5"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:13" ht="222" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="40"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="37"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="1:13" ht="229.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="41"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="38"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="39"/>
     </row>
     <row r="14" spans="1:13" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="42"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="39"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
chore(structure): Define structure of the project
</commit_message>
<xml_diff>
--- a/docs/boards/sprint_1.xlsx
+++ b/docs/boards/sprint_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157483D5-30E6-4E2C-AEB6-A528539EB311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE57EEE-6644-4D16-A2F3-164788DCEE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1789,16 +1789,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>458107</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>585107</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>182336</xdr:rowOff>
+      <xdr:rowOff>293461</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3348180</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3475180</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>2219018</xdr:rowOff>
+      <xdr:rowOff>2330143</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1813,7 +1813,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4953907" y="3878036"/>
+          <a:off x="17857107" y="4024086"/>
           <a:ext cx="2890073" cy="2036682"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -3066,16 +3066,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2571750</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2492375</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1524000</xdr:rowOff>
+      <xdr:rowOff>1635125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3092450</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3013075</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>2072640</xdr:rowOff>
+      <xdr:rowOff>2183765</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3090,7 +3090,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7067550" y="5219700"/>
+          <a:off x="19764375" y="5365750"/>
           <a:ext cx="520700" cy="548640"/>
         </a:xfrm>
         <a:custGeom>
@@ -4878,8 +4878,8 @@
   </sheetPr>
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B9" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
docs(sprint): Add complete backlog and sprint of the day
</commit_message>
<xml_diff>
--- a/docs/boards/sprint_1.xlsx
+++ b/docs/boards/sprint_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE57EEE-6644-4D16-A2F3-164788DCEE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528DC07C-E704-4558-8C32-504702813715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,10 +22,21 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sprint1!$B$1:$D$11</definedName>
     <definedName name="Type">'[1]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -872,7 +883,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>3131372</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1940151</xdr:rowOff>
+      <xdr:rowOff>1685637</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -887,8 +898,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7579359" y="2374491"/>
-          <a:ext cx="573593" cy="0"/>
+          <a:off x="23355299" y="3920427"/>
+          <a:ext cx="2890073" cy="1482846"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -1047,20 +1058,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>STATUS: Note status here</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -1080,7 +1077,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>POINTS: 0</a:t>
+            <a:t>HOURS: 0</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
@@ -1105,7 +1102,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>3809994</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1088555</xdr:rowOff>
+      <xdr:rowOff>438727</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1120,8 +1117,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8151301" y="2376335"/>
-          <a:ext cx="2093" cy="198120"/>
+          <a:off x="24033921" y="5926331"/>
+          <a:ext cx="2890073" cy="1093305"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -1287,30 +1284,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>STATUS: Note status here</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>POINTS: 0</a:t>
+            <a:t>HOURS: 0</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
@@ -1334,8 +1308,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>3092720</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>302260</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2597727</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1350,8 +1324,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7540707" y="2573020"/>
-          <a:ext cx="611693" cy="198120"/>
+          <a:off x="23316647" y="8003309"/>
+          <a:ext cx="2890073" cy="1175327"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -1517,30 +1491,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>STATUS: Note status here</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>POINTS: 0</a:t>
+            <a:t>HOURS: 0</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
@@ -1565,7 +1516,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>3797294</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>2401073</xdr:rowOff>
+      <xdr:rowOff>1881909</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1580,8 +1531,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8153841" y="2774453"/>
-          <a:ext cx="2093" cy="0"/>
+          <a:off x="24021221" y="10107895"/>
+          <a:ext cx="2890073" cy="1218196"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -1750,10 +1701,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>STATUS: Note status here</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+            <a:t>HOURS: 0</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -1762,27 +1711,6 @@
             <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>POINTS: 0</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -1790,15 +1718,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>585107</xdr:colOff>
+      <xdr:colOff>585108</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>293461</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3475180</xdr:colOff>
+      <xdr:colOff>3222626</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>2330143</xdr:rowOff>
+      <xdr:rowOff>2317750</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1813,8 +1741,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17857107" y="4024086"/>
-          <a:ext cx="2890073" cy="2036682"/>
+          <a:off x="17857108" y="4024086"/>
+          <a:ext cx="2637518" cy="2024289"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -2052,16 +1980,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>698090</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>563069</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>210165</xdr:rowOff>
+      <xdr:rowOff>908999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3588163</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>2687782</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3453142</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>529116</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2076,8 +2004,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9442040" y="3905865"/>
-          <a:ext cx="2890073" cy="2477617"/>
+          <a:off x="17816353" y="4614725"/>
+          <a:ext cx="2890073" cy="2475612"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -2309,16 +2237,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>399738</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>2335968</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>594773</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1524074</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3289811</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1956427</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3484846</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1135461</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2333,8 +2261,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4896787" y="8906657"/>
-          <a:ext cx="2890073" cy="2481081"/>
+          <a:off x="17821416" y="5211610"/>
+          <a:ext cx="2890073" cy="2468887"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -2566,16 +2494,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>478971</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>587828</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>2691495</xdr:rowOff>
+      <xdr:rowOff>2203906</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3369044</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3477901</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2138135</xdr:rowOff>
+      <xdr:rowOff>1650546</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2590,7 +2518,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4974771" y="6387195"/>
+          <a:off x="17814471" y="5891442"/>
           <a:ext cx="2890073" cy="2304140"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -2809,16 +2737,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>602840</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>857865</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>564287</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2819563</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3492913</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>439882</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3454360</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2401580</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2833,7 +2761,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9346790" y="7411065"/>
+          <a:off x="17790930" y="6507099"/>
           <a:ext cx="2890073" cy="2439517"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -3067,22 +2995,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2492375</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1635125</xdr:rowOff>
+      <xdr:colOff>2761343</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1576614</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3013075</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>2183765</xdr:rowOff>
+      <xdr:colOff>3282043</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2125254</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Freeform 2">
+        <xdr:cNvPr id="5" name="Freeform 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3336CEA4-94E3-442C-862C-86640ADB3BC4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B7188D0-CF8F-4278-B8B8-AB7E25D14A9B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3090,7 +3018,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19764375" y="5365750"/>
+          <a:off x="19987986" y="8121650"/>
           <a:ext cx="520700" cy="548640"/>
         </a:xfrm>
         <a:custGeom>
@@ -3371,23 +3299,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2762250</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>2000250</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>498462</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2696366</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3282950</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>2548890</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3388535</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1199990</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Freeform 2">
+        <xdr:cNvPr id="3" name="Snip Single Corner Rectangle 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67C38E20-DB96-47A9-92D4-685A97414E6B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AB80519-233D-4D40-BC87-83B9669015A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3395,158 +3323,25 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11506200" y="5695950"/>
-          <a:ext cx="520700" cy="548640"/>
+          <a:off x="17775984" y="9289323"/>
+          <a:ext cx="2890073" cy="1369406"/>
         </a:xfrm>
-        <a:custGeom>
+        <a:prstGeom prst="snip1Rect">
           <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 298522 w 597046"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 630113"/>
-            <a:gd name="connsiteX1" fmla="*/ 469972 w 597046"/>
-            <a:gd name="connsiteY1" fmla="*/ 165945 h 630113"/>
-            <a:gd name="connsiteX2" fmla="*/ 419755 w 597046"/>
-            <a:gd name="connsiteY2" fmla="*/ 283286 h 630113"/>
-            <a:gd name="connsiteX3" fmla="*/ 408034 w 597046"/>
-            <a:gd name="connsiteY3" fmla="*/ 290935 h 630113"/>
-            <a:gd name="connsiteX4" fmla="*/ 435155 w 597046"/>
-            <a:gd name="connsiteY4" fmla="*/ 302783 h 630113"/>
-            <a:gd name="connsiteX5" fmla="*/ 597046 w 597046"/>
-            <a:gd name="connsiteY5" fmla="*/ 583914 h 630113"/>
-            <a:gd name="connsiteX6" fmla="*/ 0 w 597046"/>
-            <a:gd name="connsiteY6" fmla="*/ 578243 h 630113"/>
-            <a:gd name="connsiteX7" fmla="*/ 159438 w 597046"/>
-            <a:gd name="connsiteY7" fmla="*/ 309073 h 630113"/>
-            <a:gd name="connsiteX8" fmla="*/ 194733 w 597046"/>
-            <a:gd name="connsiteY8" fmla="*/ 294670 h 630113"/>
-            <a:gd name="connsiteX9" fmla="*/ 177289 w 597046"/>
-            <a:gd name="connsiteY9" fmla="*/ 283286 h 630113"/>
-            <a:gd name="connsiteX10" fmla="*/ 127072 w 597046"/>
-            <a:gd name="connsiteY10" fmla="*/ 165945 h 630113"/>
-            <a:gd name="connsiteX11" fmla="*/ 298522 w 597046"/>
-            <a:gd name="connsiteY11" fmla="*/ 0 h 630113"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX5" y="connsiteY5"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX6" y="connsiteY6"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX7" y="connsiteY7"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX8" y="connsiteY8"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX9" y="connsiteY9"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX10" y="connsiteY10"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX11" y="connsiteY11"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="597046" h="630113">
-              <a:moveTo>
-                <a:pt x="298522" y="0"/>
-              </a:moveTo>
-              <a:cubicBezTo>
-                <a:pt x="393211" y="0"/>
-                <a:pt x="469972" y="74296"/>
-                <a:pt x="469972" y="165945"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="469972" y="211769"/>
-                <a:pt x="450782" y="253256"/>
-                <a:pt x="419755" y="283286"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="408034" y="290935"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="435155" y="302783"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="525950" y="364596"/>
-                <a:pt x="526507" y="507747"/>
-                <a:pt x="597046" y="583914"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="398031" y="650070"/>
-                <a:pt x="146632" y="642511"/>
-                <a:pt x="0" y="578243"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="77087" y="502076"/>
-                <a:pt x="58410" y="371684"/>
-                <a:pt x="159438" y="309073"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="194733" y="294670"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="177289" y="283286"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="146262" y="253256"/>
-                <a:pt x="127072" y="211769"/>
-                <a:pt x="127072" y="165945"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="127072" y="74296"/>
-                <a:pt x="203833" y="0"/>
-                <a:pt x="298522" y="0"/>
-              </a:cubicBezTo>
-              <a:close/>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
+        </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="00B050"/>
+          <a:srgbClr val="E0F7F7"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
             <a:prstClr val="black">
               <a:alpha val="40000"/>
             </a:prstClr>
           </a:outerShdw>
         </a:effectLst>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-        <a:sp3d contourW="12700">
-          <a:bevelT w="38100" h="25400" prst="coolSlant"/>
-          <a:contourClr>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="65000"/>
-            </a:schemeClr>
-          </a:contourClr>
-        </a:sp3d>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -3565,7 +3360,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="b"/>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle>
           <a:defPPr>
             <a:defRPr lang="en-US"/>
@@ -3662,13 +3457,57 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>EF</a:t>
-          </a:r>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Define Backlog for the entire project</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3677,22 +3516,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2457450</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1295400</xdr:rowOff>
+      <xdr:colOff>401782</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>346364</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2978150</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1844040</xdr:rowOff>
+      <xdr:colOff>3291855</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1430433</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Freeform 2">
+        <xdr:cNvPr id="4" name="Snip Single Corner Rectangle 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B7188D0-CF8F-4278-B8B8-AB7E25D14A9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92EA1B58-EE1F-4B2F-8749-6B0884C76ADD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3700,158 +3539,25 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6953250" y="10706100"/>
-          <a:ext cx="520700" cy="548640"/>
+          <a:off x="4904509" y="4059382"/>
+          <a:ext cx="2890073" cy="1084069"/>
         </a:xfrm>
-        <a:custGeom>
+        <a:prstGeom prst="snip1Rect">
           <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 298522 w 597046"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 630113"/>
-            <a:gd name="connsiteX1" fmla="*/ 469972 w 597046"/>
-            <a:gd name="connsiteY1" fmla="*/ 165945 h 630113"/>
-            <a:gd name="connsiteX2" fmla="*/ 419755 w 597046"/>
-            <a:gd name="connsiteY2" fmla="*/ 283286 h 630113"/>
-            <a:gd name="connsiteX3" fmla="*/ 408034 w 597046"/>
-            <a:gd name="connsiteY3" fmla="*/ 290935 h 630113"/>
-            <a:gd name="connsiteX4" fmla="*/ 435155 w 597046"/>
-            <a:gd name="connsiteY4" fmla="*/ 302783 h 630113"/>
-            <a:gd name="connsiteX5" fmla="*/ 597046 w 597046"/>
-            <a:gd name="connsiteY5" fmla="*/ 583914 h 630113"/>
-            <a:gd name="connsiteX6" fmla="*/ 0 w 597046"/>
-            <a:gd name="connsiteY6" fmla="*/ 578243 h 630113"/>
-            <a:gd name="connsiteX7" fmla="*/ 159438 w 597046"/>
-            <a:gd name="connsiteY7" fmla="*/ 309073 h 630113"/>
-            <a:gd name="connsiteX8" fmla="*/ 194733 w 597046"/>
-            <a:gd name="connsiteY8" fmla="*/ 294670 h 630113"/>
-            <a:gd name="connsiteX9" fmla="*/ 177289 w 597046"/>
-            <a:gd name="connsiteY9" fmla="*/ 283286 h 630113"/>
-            <a:gd name="connsiteX10" fmla="*/ 127072 w 597046"/>
-            <a:gd name="connsiteY10" fmla="*/ 165945 h 630113"/>
-            <a:gd name="connsiteX11" fmla="*/ 298522 w 597046"/>
-            <a:gd name="connsiteY11" fmla="*/ 0 h 630113"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX5" y="connsiteY5"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX6" y="connsiteY6"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX7" y="connsiteY7"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX8" y="connsiteY8"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX9" y="connsiteY9"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX10" y="connsiteY10"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX11" y="connsiteY11"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="597046" h="630113">
-              <a:moveTo>
-                <a:pt x="298522" y="0"/>
-              </a:moveTo>
-              <a:cubicBezTo>
-                <a:pt x="393211" y="0"/>
-                <a:pt x="469972" y="74296"/>
-                <a:pt x="469972" y="165945"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="469972" y="211769"/>
-                <a:pt x="450782" y="253256"/>
-                <a:pt x="419755" y="283286"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="408034" y="290935"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="435155" y="302783"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="525950" y="364596"/>
-                <a:pt x="526507" y="507747"/>
-                <a:pt x="597046" y="583914"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="398031" y="650070"/>
-                <a:pt x="146632" y="642511"/>
-                <a:pt x="0" y="578243"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="77087" y="502076"/>
-                <a:pt x="58410" y="371684"/>
-                <a:pt x="159438" y="309073"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="194733" y="294670"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="177289" y="283286"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="146262" y="253256"/>
-                <a:pt x="127072" y="211769"/>
-                <a:pt x="127072" y="165945"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="127072" y="74296"/>
-                <a:pt x="203833" y="0"/>
-                <a:pt x="298522" y="0"/>
-              </a:cubicBezTo>
-              <a:close/>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
+        </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="00B050"/>
+          <a:srgbClr val="E0F7F7"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
             <a:prstClr val="black">
               <a:alpha val="40000"/>
             </a:prstClr>
           </a:outerShdw>
         </a:effectLst>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-        <a:sp3d contourW="12700">
-          <a:bevelT w="38100" h="25400" prst="coolSlant"/>
-          <a:contourClr>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="65000"/>
-            </a:schemeClr>
-          </a:contourClr>
-        </a:sp3d>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -3870,7 +3576,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="b"/>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle>
           <a:defPPr>
             <a:defRPr lang="en-US"/>
@@ -3967,13 +3673,48 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Lay the foundation for user interaction and game flow.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>EF</a:t>
-          </a:r>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3982,22 +3723,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2647950</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1447800</xdr:rowOff>
+      <xdr:colOff>360219</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1801091</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3168650</xdr:colOff>
+      <xdr:colOff>3250292</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1996440</xdr:rowOff>
+      <xdr:rowOff>1995054</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Freeform 2">
+        <xdr:cNvPr id="6" name="Snip Single Corner Rectangle 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C30CE06-CE9B-47D4-A4B2-F47F985F49F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{553683D0-0AE0-4F86-9649-EFC64AD19EEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4005,158 +3746,25 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7143750" y="8001000"/>
-          <a:ext cx="520700" cy="548640"/>
+          <a:off x="4862946" y="5514109"/>
+          <a:ext cx="2890073" cy="3048000"/>
         </a:xfrm>
-        <a:custGeom>
+        <a:prstGeom prst="snip1Rect">
           <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 298522 w 597046"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 630113"/>
-            <a:gd name="connsiteX1" fmla="*/ 469972 w 597046"/>
-            <a:gd name="connsiteY1" fmla="*/ 165945 h 630113"/>
-            <a:gd name="connsiteX2" fmla="*/ 419755 w 597046"/>
-            <a:gd name="connsiteY2" fmla="*/ 283286 h 630113"/>
-            <a:gd name="connsiteX3" fmla="*/ 408034 w 597046"/>
-            <a:gd name="connsiteY3" fmla="*/ 290935 h 630113"/>
-            <a:gd name="connsiteX4" fmla="*/ 435155 w 597046"/>
-            <a:gd name="connsiteY4" fmla="*/ 302783 h 630113"/>
-            <a:gd name="connsiteX5" fmla="*/ 597046 w 597046"/>
-            <a:gd name="connsiteY5" fmla="*/ 583914 h 630113"/>
-            <a:gd name="connsiteX6" fmla="*/ 0 w 597046"/>
-            <a:gd name="connsiteY6" fmla="*/ 578243 h 630113"/>
-            <a:gd name="connsiteX7" fmla="*/ 159438 w 597046"/>
-            <a:gd name="connsiteY7" fmla="*/ 309073 h 630113"/>
-            <a:gd name="connsiteX8" fmla="*/ 194733 w 597046"/>
-            <a:gd name="connsiteY8" fmla="*/ 294670 h 630113"/>
-            <a:gd name="connsiteX9" fmla="*/ 177289 w 597046"/>
-            <a:gd name="connsiteY9" fmla="*/ 283286 h 630113"/>
-            <a:gd name="connsiteX10" fmla="*/ 127072 w 597046"/>
-            <a:gd name="connsiteY10" fmla="*/ 165945 h 630113"/>
-            <a:gd name="connsiteX11" fmla="*/ 298522 w 597046"/>
-            <a:gd name="connsiteY11" fmla="*/ 0 h 630113"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX5" y="connsiteY5"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX6" y="connsiteY6"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX7" y="connsiteY7"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX8" y="connsiteY8"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX9" y="connsiteY9"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX10" y="connsiteY10"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX11" y="connsiteY11"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="597046" h="630113">
-              <a:moveTo>
-                <a:pt x="298522" y="0"/>
-              </a:moveTo>
-              <a:cubicBezTo>
-                <a:pt x="393211" y="0"/>
-                <a:pt x="469972" y="74296"/>
-                <a:pt x="469972" y="165945"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="469972" y="211769"/>
-                <a:pt x="450782" y="253256"/>
-                <a:pt x="419755" y="283286"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="408034" y="290935"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="435155" y="302783"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="525950" y="364596"/>
-                <a:pt x="526507" y="507747"/>
-                <a:pt x="597046" y="583914"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="398031" y="650070"/>
-                <a:pt x="146632" y="642511"/>
-                <a:pt x="0" y="578243"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="77087" y="502076"/>
-                <a:pt x="58410" y="371684"/>
-                <a:pt x="159438" y="309073"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="194733" y="294670"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="177289" y="283286"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="146262" y="253256"/>
-                <a:pt x="127072" y="211769"/>
-                <a:pt x="127072" y="165945"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="127072" y="74296"/>
-                <a:pt x="203833" y="0"/>
-                <a:pt x="298522" y="0"/>
-              </a:cubicBezTo>
-              <a:close/>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
+        </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="00B050"/>
+          <a:srgbClr val="E0F7F7"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
             <a:prstClr val="black">
               <a:alpha val="40000"/>
             </a:prstClr>
           </a:outerShdw>
         </a:effectLst>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-        <a:sp3d contourW="12700">
-          <a:bevelT w="38100" h="25400" prst="coolSlant"/>
-          <a:contourClr>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="65000"/>
-            </a:schemeClr>
-          </a:contourClr>
-        </a:sp3d>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -4175,7 +3783,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="b"/>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle>
           <a:defPPr>
             <a:defRPr lang="en-US"/>
@@ -4272,13 +3880,91 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Establish the building blocks of your game logic</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1400">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- Define simple case classes for Player, World, and GameState in the domain layer.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- Add basic properties (e.g., player name, world size, game status).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- Write minimal unit tests for these models (if you have time).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>EF</a:t>
-          </a:r>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 0.30</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4286,23 +3972,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2876550</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>443345</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2514600</xdr:rowOff>
+      <xdr:rowOff>2466109</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3397250</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3333418</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>205740</xdr:rowOff>
+      <xdr:rowOff>872836</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Freeform 2">
+        <xdr:cNvPr id="7" name="Snip Single Corner Rectangle 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82B115B4-DF55-4A12-82E3-11CB374D6763}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82CC7BC2-29A3-42A8-B11A-F0A6BD3B89AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4310,158 +3996,25 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11620500" y="9067800"/>
-          <a:ext cx="520700" cy="548640"/>
+          <a:off x="4946072" y="9033164"/>
+          <a:ext cx="2890073" cy="1260763"/>
         </a:xfrm>
-        <a:custGeom>
+        <a:prstGeom prst="snip1Rect">
           <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 298522 w 597046"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 630113"/>
-            <a:gd name="connsiteX1" fmla="*/ 469972 w 597046"/>
-            <a:gd name="connsiteY1" fmla="*/ 165945 h 630113"/>
-            <a:gd name="connsiteX2" fmla="*/ 419755 w 597046"/>
-            <a:gd name="connsiteY2" fmla="*/ 283286 h 630113"/>
-            <a:gd name="connsiteX3" fmla="*/ 408034 w 597046"/>
-            <a:gd name="connsiteY3" fmla="*/ 290935 h 630113"/>
-            <a:gd name="connsiteX4" fmla="*/ 435155 w 597046"/>
-            <a:gd name="connsiteY4" fmla="*/ 302783 h 630113"/>
-            <a:gd name="connsiteX5" fmla="*/ 597046 w 597046"/>
-            <a:gd name="connsiteY5" fmla="*/ 583914 h 630113"/>
-            <a:gd name="connsiteX6" fmla="*/ 0 w 597046"/>
-            <a:gd name="connsiteY6" fmla="*/ 578243 h 630113"/>
-            <a:gd name="connsiteX7" fmla="*/ 159438 w 597046"/>
-            <a:gd name="connsiteY7" fmla="*/ 309073 h 630113"/>
-            <a:gd name="connsiteX8" fmla="*/ 194733 w 597046"/>
-            <a:gd name="connsiteY8" fmla="*/ 294670 h 630113"/>
-            <a:gd name="connsiteX9" fmla="*/ 177289 w 597046"/>
-            <a:gd name="connsiteY9" fmla="*/ 283286 h 630113"/>
-            <a:gd name="connsiteX10" fmla="*/ 127072 w 597046"/>
-            <a:gd name="connsiteY10" fmla="*/ 165945 h 630113"/>
-            <a:gd name="connsiteX11" fmla="*/ 298522 w 597046"/>
-            <a:gd name="connsiteY11" fmla="*/ 0 h 630113"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX5" y="connsiteY5"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX6" y="connsiteY6"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX7" y="connsiteY7"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX8" y="connsiteY8"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX9" y="connsiteY9"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX10" y="connsiteY10"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX11" y="connsiteY11"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="597046" h="630113">
-              <a:moveTo>
-                <a:pt x="298522" y="0"/>
-              </a:moveTo>
-              <a:cubicBezTo>
-                <a:pt x="393211" y="0"/>
-                <a:pt x="469972" y="74296"/>
-                <a:pt x="469972" y="165945"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="469972" y="211769"/>
-                <a:pt x="450782" y="253256"/>
-                <a:pt x="419755" y="283286"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="408034" y="290935"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="435155" y="302783"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="525950" y="364596"/>
-                <a:pt x="526507" y="507747"/>
-                <a:pt x="597046" y="583914"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="398031" y="650070"/>
-                <a:pt x="146632" y="642511"/>
-                <a:pt x="0" y="578243"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="77087" y="502076"/>
-                <a:pt x="58410" y="371684"/>
-                <a:pt x="159438" y="309073"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="194733" y="294670"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="177289" y="283286"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="146262" y="253256"/>
-                <a:pt x="127072" y="211769"/>
-                <a:pt x="127072" y="165945"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="127072" y="74296"/>
-                <a:pt x="203833" y="0"/>
-                <a:pt x="298522" y="0"/>
-              </a:cubicBezTo>
-              <a:close/>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
+        </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="00B050"/>
+          <a:srgbClr val="E0F7F7"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
             <a:prstClr val="black">
               <a:alpha val="40000"/>
             </a:prstClr>
           </a:outerShdw>
         </a:effectLst>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-        <a:sp3d contourW="12700">
-          <a:bevelT w="38100" h="25400" prst="coolSlant"/>
-          <a:contourClr>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="65000"/>
-            </a:schemeClr>
-          </a:contourClr>
-        </a:sp3d>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -4480,7 +4033,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="b"/>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle>
           <a:defPPr>
             <a:defRPr lang="en-US"/>
@@ -4577,13 +4130,44 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Keep your documentation and sprint board up to date.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>EF</a:t>
-          </a:r>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 0.30</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4876,10 +4460,10 @@
     <tabColor theme="3" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="34" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4894,21 +4478,21 @@
     <col min="12" max="16384" width="11.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="33" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="33" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36"/>
       <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="34"/>
     </row>
-    <row r="2" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:13" s="30" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="30" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="32" t="s">
         <v>1</v>
       </c>
@@ -4927,7 +4511,7 @@
       <c r="I3" s="31"/>
       <c r="J3" s="31"/>
     </row>
-    <row r="4" spans="1:13" s="22" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="22" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="29">
         <v>45817</v>
       </c>
@@ -4946,7 +4530,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="23"/>
     </row>
-    <row r="5" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="21" t="s">
         <v>5</v>
       </c>
@@ -4955,7 +4539,7 @@
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
         <v>15</v>
       </c>
@@ -4963,7 +4547,7 @@
       <c r="E6" s="2"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B7" s="19" t="s">
         <v>6</v>
       </c>
@@ -4972,7 +4556,7 @@
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" s="10" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B8" s="17" t="s">
         <v>7</v>
       </c>
@@ -4995,7 +4579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="44"/>
       <c r="C9" s="41"/>
       <c r="D9" s="38"/>
@@ -5004,7 +4588,7 @@
       <c r="H9" s="9"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="45"/>
       <c r="C10" s="42"/>
       <c r="D10" s="39"/>
@@ -5014,7 +4598,7 @@
       <c r="J10" s="6"/>
       <c r="M10" s="37"/>
     </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="46"/>
       <c r="C11" s="43"/>
       <c r="D11" s="40"/>
@@ -5022,20 +4606,21 @@
       <c r="F11" s="40"/>
       <c r="H11" s="5"/>
       <c r="J11" s="4"/>
+      <c r="O11" s="37"/>
     </row>
-    <row r="12" spans="1:13" ht="222" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="41"/>
       <c r="D12" s="38"/>
       <c r="E12" s="41"/>
       <c r="F12" s="38"/>
     </row>
-    <row r="13" spans="1:13" ht="229.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="229.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="42"/>
       <c r="D13" s="39"/>
       <c r="E13" s="42"/>
       <c r="F13" s="39"/>
     </row>
-    <row r="14" spans="1:13" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="43"/>
       <c r="D14" s="40"/>
       <c r="E14" s="43"/>

</xml_diff>

<commit_message>
docs(sprint): Move tasks done to complete
</commit_message>
<xml_diff>
--- a/docs/boards/sprint_1.xlsx
+++ b/docs/boards/sprint_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528DC07C-E704-4558-8C32-504702813715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC20719F-C31D-4FEE-98D8-D9BB8794A722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,6 +520,15 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -536,15 +545,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3300,22 +3300,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>498462</xdr:colOff>
+      <xdr:colOff>577628</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2696366</xdr:rowOff>
+      <xdr:rowOff>2667532</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3388535</xdr:colOff>
+      <xdr:colOff>3467701</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1199990</xdr:rowOff>
+      <xdr:rowOff>1299476</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Snip Single Corner Rectangle 20">
+        <xdr:cNvPr id="4" name="Snip Single Corner Rectangle 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AB80519-233D-4D40-BC87-83B9669015A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92EA1B58-EE1F-4B2F-8749-6B0884C76ADD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3323,8 +3323,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17775984" y="9289323"/>
-          <a:ext cx="2890073" cy="1369406"/>
+          <a:off x="17845720" y="9244178"/>
+          <a:ext cx="2890073" cy="1492375"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -3458,19 +3458,31 @@
         </a:lstStyle>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
+            <a:rPr lang="it-IT" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Define Backlog for the entire project</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Create initial project documentation and architecture overview</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1200" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400"/>
+            <a:t>.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -3480,6 +3492,18 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -3488,50 +3512,29 @@
             <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>HOURS: 1</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>401782</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>346364</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>591876</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>670323</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3291855</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1430433</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3481949</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1826123</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Snip Single Corner Rectangle 20">
+        <xdr:cNvPr id="6" name="Snip Single Corner Rectangle 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92EA1B58-EE1F-4B2F-8749-6B0884C76ADD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{553683D0-0AE0-4F86-9649-EFC64AD19EEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3539,8 +3542,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4904509" y="4059382"/>
-          <a:ext cx="2890073" cy="1084069"/>
+          <a:off x="17832126" y="10081023"/>
+          <a:ext cx="2890073" cy="1155800"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -3674,18 +3677,46 @@
         </a:lstStyle>
         <a:p>
           <a:r>
-            <a:rPr lang="it-IT" sz="1400" b="1">
+            <a:rPr lang="it-IT" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-            </a:rPr>
-            <a:t>Lay the foundation for user interaction and game flow.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1400"/>
-            <a:t>.</a:t>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Design and document core game loop.</a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 0.30</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
@@ -3695,50 +3726,29 @@
             <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>HOURS: 1</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>360219</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1801091</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>580009</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1314443</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3250292</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1995054</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3470082</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2586952</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Snip Single Corner Rectangle 20">
+        <xdr:cNvPr id="7" name="Snip Single Corner Rectangle 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{553683D0-0AE0-4F86-9649-EFC64AD19EEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82CC7BC2-29A3-42A8-B11A-F0A6BD3B89AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3746,8 +3756,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4862946" y="5514109"/>
-          <a:ext cx="2890073" cy="3048000"/>
+          <a:off x="17820259" y="10725143"/>
+          <a:ext cx="2890073" cy="1272509"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -3881,24 +3891,18 @@
         </a:lstStyle>
         <a:p>
           <a:r>
-            <a:rPr lang="it-IT" sz="1400" b="1">
+            <a:rPr lang="it-IT" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-            </a:rPr>
-            <a:t>Establish the building blocks of your game logic</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1400">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="it-IT" sz="1400">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Define main entry point (e.g., CliApp.scala).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="1" i="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -3907,42 +3911,14 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1400">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- Define simple case classes for Player, World, and GameState in the domain layer.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1400">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- Add basic properties (e.g., player name, world size, game status).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1400">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- Write minimal unit tests for these models (if you have time).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
+          <a:endParaRPr lang="en-US" sz="1400" kern="1200" baseline="0">
             <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:effectLst/>
             <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -3972,23 +3948,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>443345</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>2466109</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>496956</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>546652</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3333418</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>872836</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3387029</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1764848</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Snip Single Corner Rectangle 20">
+        <xdr:cNvPr id="8" name="Snip Single Corner Rectangle 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82CC7BC2-29A3-42A8-B11A-F0A6BD3B89AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11545847-466F-4B5E-81D6-D536DE2D8D1B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3996,8 +3972,1759 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4946072" y="9033164"/>
-          <a:ext cx="2890073" cy="1260763"/>
+          <a:off x="745434" y="4273826"/>
+          <a:ext cx="2890073" cy="1218196"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Define GameState management</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>430696</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1888435</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3320769</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>240848</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Snip Single Corner Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB358556-6B3D-42CD-AC78-CE50E6DD5B6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="679174" y="5615609"/>
+          <a:ext cx="2890073" cy="1218196"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Implement error handling and logging infrastructure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>450574</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>367747</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3340647</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1585943</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Snip Single Corner Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B845277E-3EC1-4CA5-B4AD-C8357EF4B469}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="699052" y="6960704"/>
+          <a:ext cx="2890073" cy="1218196"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Specify interfaces/traits for world generation</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>530087</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2170043</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3420160</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>479588</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Snip Single Corner Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AB2B739-A871-43B9-96D1-2947BD6EC52B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="778565" y="8763000"/>
+          <a:ext cx="2890073" cy="1175327"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="F6E9FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Define Player model and attributes</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" kern="1200" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1.30</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>516835</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>765313</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3406908</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1940640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Snip Single Corner Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78E54BF4-F4F6-4DEA-BC13-0F5C893338BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="765313" y="10224052"/>
+          <a:ext cx="2890073" cy="1175327"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="F6E9FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Define World model and structure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" kern="1200" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1.30</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>453887</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>89451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3343960</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1905000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Snip Single Corner Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A667416-DA8F-4478-A3D7-CAF37E76DF01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="702365" y="12413973"/>
+          <a:ext cx="2890073" cy="1815549"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Set up configuration management (game settings, environment variables)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="it-IT" sz="1400" kern="1200" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 0.30</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>443948</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2199860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3334021</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>977348</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Snip Single Corner Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3A11A3B-F27C-4D68-8704-CEE7DBFA0CED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="692426" y="14524382"/>
+          <a:ext cx="2890073" cy="1593575"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Specify interfaces/traits for player actions and game events</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1.30</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>496957</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1159564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3387030</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>2753139</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Snip Single Corner Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB378F22-8EA5-481D-A46E-97A8B2E9CA6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="745435" y="16300173"/>
+          <a:ext cx="2890073" cy="1593575"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="114300" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Implement core domain logic for turn progression, win/loss conditions</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>595049</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2045290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3485122</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>551845</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Snip Single Corner Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5C3825D-6B38-6959-E672-10BD690E3599}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17835299" y="11455990"/>
+          <a:ext cx="2890073" cy="1364055"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -4131,26 +5858,7 @@
         </a:lstStyle>
         <a:p>
           <a:r>
-            <a:rPr lang="it-IT" sz="1400" b="1">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Keep your documentation and sprint board up to date.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" b="1">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+            <a:rPr lang="en-US" sz="1400" b="1" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -4159,8 +5867,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>HOURS: 0.30</a:t>
-          </a:r>
+            <a:t>Define Backlog for the entire project</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -4168,6 +5878,341 @@
             <a:effectLst/>
             <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>HOURS: 1</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2766749</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2673940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3287449</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>365080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Freeform 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07509ECE-1496-4F0A-BF42-027A7AABCCCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20006999" y="12084640"/>
+          <a:ext cx="520700" cy="548640"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 298522 w 597046"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 630113"/>
+            <a:gd name="connsiteX1" fmla="*/ 469972 w 597046"/>
+            <a:gd name="connsiteY1" fmla="*/ 165945 h 630113"/>
+            <a:gd name="connsiteX2" fmla="*/ 419755 w 597046"/>
+            <a:gd name="connsiteY2" fmla="*/ 283286 h 630113"/>
+            <a:gd name="connsiteX3" fmla="*/ 408034 w 597046"/>
+            <a:gd name="connsiteY3" fmla="*/ 290935 h 630113"/>
+            <a:gd name="connsiteX4" fmla="*/ 435155 w 597046"/>
+            <a:gd name="connsiteY4" fmla="*/ 302783 h 630113"/>
+            <a:gd name="connsiteX5" fmla="*/ 597046 w 597046"/>
+            <a:gd name="connsiteY5" fmla="*/ 583914 h 630113"/>
+            <a:gd name="connsiteX6" fmla="*/ 0 w 597046"/>
+            <a:gd name="connsiteY6" fmla="*/ 578243 h 630113"/>
+            <a:gd name="connsiteX7" fmla="*/ 159438 w 597046"/>
+            <a:gd name="connsiteY7" fmla="*/ 309073 h 630113"/>
+            <a:gd name="connsiteX8" fmla="*/ 194733 w 597046"/>
+            <a:gd name="connsiteY8" fmla="*/ 294670 h 630113"/>
+            <a:gd name="connsiteX9" fmla="*/ 177289 w 597046"/>
+            <a:gd name="connsiteY9" fmla="*/ 283286 h 630113"/>
+            <a:gd name="connsiteX10" fmla="*/ 127072 w 597046"/>
+            <a:gd name="connsiteY10" fmla="*/ 165945 h 630113"/>
+            <a:gd name="connsiteX11" fmla="*/ 298522 w 597046"/>
+            <a:gd name="connsiteY11" fmla="*/ 0 h 630113"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="597046" h="630113">
+              <a:moveTo>
+                <a:pt x="298522" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="393211" y="0"/>
+                <a:pt x="469972" y="74296"/>
+                <a:pt x="469972" y="165945"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="469972" y="211769"/>
+                <a:pt x="450782" y="253256"/>
+                <a:pt x="419755" y="283286"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="408034" y="290935"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="435155" y="302783"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="525950" y="364596"/>
+                <a:pt x="526507" y="507747"/>
+                <a:pt x="597046" y="583914"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="398031" y="650070"/>
+                <a:pt x="146632" y="642511"/>
+                <a:pt x="0" y="578243"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="77087" y="502076"/>
+                <a:pt x="58410" y="371684"/>
+                <a:pt x="159438" y="309073"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="194733" y="294670"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="177289" y="283286"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="146262" y="253256"/>
+                <a:pt x="127072" y="211769"/>
+                <a:pt x="127072" y="165945"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="127072" y="74296"/>
+                <a:pt x="203833" y="0"/>
+                <a:pt x="298522" y="0"/>
+              </a:cubicBezTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="threePt" dir="t"/>
+        </a:scene3d>
+        <a:sp3d contourW="12700">
+          <a:bevelT w="38100" h="25400" prst="coolSlant"/>
+          <a:contourClr>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="b"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>EF</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4462,8 +6507,8 @@
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="34" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4580,58 +6625,62 @@
       </c>
     </row>
     <row r="9" spans="1:15" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="44"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="41"/>
       <c r="H9" s="9"/>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:15" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="45"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="42"/>
       <c r="H10" s="7"/>
       <c r="J10" s="6"/>
       <c r="M10" s="37"/>
     </row>
     <row r="11" spans="1:15" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="46"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="43"/>
       <c r="H11" s="5"/>
       <c r="J11" s="4"/>
       <c r="O11" s="37"/>
     </row>
     <row r="12" spans="1:15" ht="222" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="41"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="38"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="41"/>
     </row>
     <row r="13" spans="1:15" ht="229.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="42"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="39"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="42"/>
     </row>
     <row r="14" spans="1:15" ht="264.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="43"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="40"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="F12:F14"/>
-    <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>

</xml_diff>

<commit_message>
refactor: Refactor in enums definition for direction
</commit_message>
<xml_diff>
--- a/docs/boards/sprint_1.xlsx
+++ b/docs/boards/sprint_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC20719F-C31D-4FEE-98D8-D9BB8794A722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859D8324-4BB0-413D-863D-EB4877279A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3948,16 +3948,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>496956</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>801756</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>546652</xdr:rowOff>
+      <xdr:rowOff>348532</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3387029</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3691829</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1764848</xdr:rowOff>
+      <xdr:rowOff>1566728</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3972,7 +3972,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="745434" y="4273826"/>
+          <a:off x="5312796" y="4082332"/>
           <a:ext cx="2890073" cy="1218196"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -4166,16 +4166,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>430696</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>705016</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1888435</xdr:rowOff>
+      <xdr:rowOff>1827475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3320769</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3595089</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>240848</xdr:rowOff>
+      <xdr:rowOff>179888</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4190,8 +4190,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="679174" y="5615609"/>
-          <a:ext cx="2890073" cy="1218196"/>
+          <a:off x="5216056" y="5561275"/>
+          <a:ext cx="2890073" cy="1217533"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -4384,16 +4384,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>450574</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>755374</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>367747</xdr:rowOff>
+      <xdr:rowOff>337267</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3340647</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3645447</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1585943</xdr:rowOff>
+      <xdr:rowOff>1555463</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4408,7 +4408,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="699052" y="6960704"/>
+          <a:off x="5266414" y="6936187"/>
           <a:ext cx="2890073" cy="1218196"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -6507,8 +6507,8 @@
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="50" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6564,7 +6564,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="27">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
docs(sprint): Update kanban board
</commit_message>
<xml_diff>
--- a/docs/boards/sprint_1.xlsx
+++ b/docs/boards/sprint_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF4AA61-D683-45B5-98B0-927631D3DF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6501CE-B2C5-4D9B-8D65-77C041B3D1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2748" yWindow="1812" windowWidth="17676" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="2" r:id="rId1"/>
@@ -100,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +242,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -415,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -545,6 +552,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4383,16 +4399,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>447261</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>463826</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726042</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>928461</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3337334</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1639153</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3616115</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>2103788</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4407,7 +4423,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4953000" y="4191000"/>
+          <a:off x="18010432" y="16075534"/>
           <a:ext cx="2890073" cy="1175327"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -4609,15 +4625,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>732182</xdr:colOff>
+      <xdr:colOff>750767</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>881269</xdr:rowOff>
+      <xdr:rowOff>1606098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3622255</xdr:colOff>
+      <xdr:colOff>3640840</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>2056596</xdr:rowOff>
+      <xdr:rowOff>2781425</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4632,7 +4648,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18009704" y="16021878"/>
+          <a:off x="18035157" y="16753171"/>
           <a:ext cx="2890073" cy="1175327"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -4833,16 +4849,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>420757</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1944755</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>680953</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>30462</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3310830</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>894521</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3571026</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1842374</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4857,8 +4873,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4926496" y="5671929"/>
-          <a:ext cx="2890073" cy="1815549"/>
+          <a:off x="17965343" y="18095438"/>
+          <a:ext cx="2890073" cy="1811912"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
           <a:avLst/>
@@ -5050,16 +5066,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>377687</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1139686</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>675054</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1381296</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3267760</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>2733261</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3565127</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>2974871</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5074,7 +5090,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4883426" y="7732643"/>
+          <a:off x="17959444" y="19446272"/>
           <a:ext cx="2890073" cy="1593575"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -5262,16 +5278,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>314740</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>132520</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>686449</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>2325593</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3204813</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1726095</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3576522</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>146339</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5286,7 +5302,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4820479" y="9591259"/>
+          <a:off x="17970839" y="20390569"/>
           <a:ext cx="2890073" cy="1593575"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -6243,6 +6259,616 @@
         <a:xfrm>
           <a:off x="20010783" y="14991522"/>
           <a:ext cx="520700" cy="548640"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 298522 w 597046"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 630113"/>
+            <a:gd name="connsiteX1" fmla="*/ 469972 w 597046"/>
+            <a:gd name="connsiteY1" fmla="*/ 165945 h 630113"/>
+            <a:gd name="connsiteX2" fmla="*/ 419755 w 597046"/>
+            <a:gd name="connsiteY2" fmla="*/ 283286 h 630113"/>
+            <a:gd name="connsiteX3" fmla="*/ 408034 w 597046"/>
+            <a:gd name="connsiteY3" fmla="*/ 290935 h 630113"/>
+            <a:gd name="connsiteX4" fmla="*/ 435155 w 597046"/>
+            <a:gd name="connsiteY4" fmla="*/ 302783 h 630113"/>
+            <a:gd name="connsiteX5" fmla="*/ 597046 w 597046"/>
+            <a:gd name="connsiteY5" fmla="*/ 583914 h 630113"/>
+            <a:gd name="connsiteX6" fmla="*/ 0 w 597046"/>
+            <a:gd name="connsiteY6" fmla="*/ 578243 h 630113"/>
+            <a:gd name="connsiteX7" fmla="*/ 159438 w 597046"/>
+            <a:gd name="connsiteY7" fmla="*/ 309073 h 630113"/>
+            <a:gd name="connsiteX8" fmla="*/ 194733 w 597046"/>
+            <a:gd name="connsiteY8" fmla="*/ 294670 h 630113"/>
+            <a:gd name="connsiteX9" fmla="*/ 177289 w 597046"/>
+            <a:gd name="connsiteY9" fmla="*/ 283286 h 630113"/>
+            <a:gd name="connsiteX10" fmla="*/ 127072 w 597046"/>
+            <a:gd name="connsiteY10" fmla="*/ 165945 h 630113"/>
+            <a:gd name="connsiteX11" fmla="*/ 298522 w 597046"/>
+            <a:gd name="connsiteY11" fmla="*/ 0 h 630113"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="597046" h="630113">
+              <a:moveTo>
+                <a:pt x="298522" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="393211" y="0"/>
+                <a:pt x="469972" y="74296"/>
+                <a:pt x="469972" y="165945"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="469972" y="211769"/>
+                <a:pt x="450782" y="253256"/>
+                <a:pt x="419755" y="283286"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="408034" y="290935"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="435155" y="302783"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="525950" y="364596"/>
+                <a:pt x="526507" y="507747"/>
+                <a:pt x="597046" y="583914"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="398031" y="650070"/>
+                <a:pt x="146632" y="642511"/>
+                <a:pt x="0" y="578243"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="77087" y="502076"/>
+                <a:pt x="58410" y="371684"/>
+                <a:pt x="159438" y="309073"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="194733" y="294670"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="177289" y="283286"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="146262" y="253256"/>
+                <a:pt x="127072" y="211769"/>
+                <a:pt x="127072" y="165945"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="127072" y="74296"/>
+                <a:pt x="203833" y="0"/>
+                <a:pt x="298522" y="0"/>
+              </a:cubicBezTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="threePt" dir="t"/>
+        </a:scene3d>
+        <a:sp3d contourW="12700">
+          <a:bevelT w="38100" h="25400" prst="coolSlant"/>
+          <a:contourClr>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="b"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>EF</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2850913</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>2052146</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3371613</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>2609674</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Freeform 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDD3AD4B-DB6C-4BDC-8292-3F85063FAF48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20135303" y="17199219"/>
+          <a:ext cx="520700" cy="557528"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 298522 w 597046"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 630113"/>
+            <a:gd name="connsiteX1" fmla="*/ 469972 w 597046"/>
+            <a:gd name="connsiteY1" fmla="*/ 165945 h 630113"/>
+            <a:gd name="connsiteX2" fmla="*/ 419755 w 597046"/>
+            <a:gd name="connsiteY2" fmla="*/ 283286 h 630113"/>
+            <a:gd name="connsiteX3" fmla="*/ 408034 w 597046"/>
+            <a:gd name="connsiteY3" fmla="*/ 290935 h 630113"/>
+            <a:gd name="connsiteX4" fmla="*/ 435155 w 597046"/>
+            <a:gd name="connsiteY4" fmla="*/ 302783 h 630113"/>
+            <a:gd name="connsiteX5" fmla="*/ 597046 w 597046"/>
+            <a:gd name="connsiteY5" fmla="*/ 583914 h 630113"/>
+            <a:gd name="connsiteX6" fmla="*/ 0 w 597046"/>
+            <a:gd name="connsiteY6" fmla="*/ 578243 h 630113"/>
+            <a:gd name="connsiteX7" fmla="*/ 159438 w 597046"/>
+            <a:gd name="connsiteY7" fmla="*/ 309073 h 630113"/>
+            <a:gd name="connsiteX8" fmla="*/ 194733 w 597046"/>
+            <a:gd name="connsiteY8" fmla="*/ 294670 h 630113"/>
+            <a:gd name="connsiteX9" fmla="*/ 177289 w 597046"/>
+            <a:gd name="connsiteY9" fmla="*/ 283286 h 630113"/>
+            <a:gd name="connsiteX10" fmla="*/ 127072 w 597046"/>
+            <a:gd name="connsiteY10" fmla="*/ 165945 h 630113"/>
+            <a:gd name="connsiteX11" fmla="*/ 298522 w 597046"/>
+            <a:gd name="connsiteY11" fmla="*/ 0 h 630113"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="597046" h="630113">
+              <a:moveTo>
+                <a:pt x="298522" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="393211" y="0"/>
+                <a:pt x="469972" y="74296"/>
+                <a:pt x="469972" y="165945"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="469972" y="211769"/>
+                <a:pt x="450782" y="253256"/>
+                <a:pt x="419755" y="283286"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="408034" y="290935"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="435155" y="302783"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="525950" y="364596"/>
+                <a:pt x="526507" y="507747"/>
+                <a:pt x="597046" y="583914"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="398031" y="650070"/>
+                <a:pt x="146632" y="642511"/>
+                <a:pt x="0" y="578243"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="77087" y="502076"/>
+                <a:pt x="58410" y="371684"/>
+                <a:pt x="159438" y="309073"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="194733" y="294670"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="177289" y="283286"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="146262" y="253256"/>
+                <a:pt x="127072" y="211769"/>
+                <a:pt x="127072" y="165945"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="127072" y="74296"/>
+                <a:pt x="203833" y="0"/>
+                <a:pt x="298522" y="0"/>
+              </a:cubicBezTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="threePt" dir="t"/>
+        </a:scene3d>
+        <a:sp3d contourW="12700">
+          <a:bevelT w="38100" h="25400" prst="coolSlant"/>
+          <a:contourClr>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="b"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>EF</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2732049</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>3178097</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3252749</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>167235</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Freeform 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA9065D3-C049-4292-B4E0-09B80B1E2BBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20016439" y="21243073"/>
+          <a:ext cx="520700" cy="557528"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6809,8 +7435,8 @@
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="46" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="41" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6930,7 +7556,7 @@
       <c r="B9" s="38"/>
       <c r="C9" s="44"/>
       <c r="D9" s="41"/>
-      <c r="E9" s="44"/>
+      <c r="E9" s="47"/>
       <c r="F9" s="41"/>
       <c r="H9" s="9"/>
       <c r="J9" s="8"/>
@@ -6939,7 +7565,7 @@
       <c r="B10" s="39"/>
       <c r="C10" s="45"/>
       <c r="D10" s="42"/>
-      <c r="E10" s="45"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="42"/>
       <c r="H10" s="7"/>
       <c r="J10" s="6"/>
@@ -6949,7 +7575,7 @@
       <c r="B11" s="40"/>
       <c r="C11" s="46"/>
       <c r="D11" s="43"/>
-      <c r="E11" s="46"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="43"/>
       <c r="H11" s="5"/>
       <c r="J11" s="4"/>
@@ -6990,7 +7616,7 @@
     <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup scale="74" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="74" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>